<commit_message>
Tabela com descrição das colunas / windows 07112024
</commit_message>
<xml_diff>
--- a/Tabela Variaveis Analises Pe de Meia.xlsx
+++ b/Tabela Variaveis Analises Pe de Meia.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f97fb756bfb044a9/1. Educacao/2. Academia/3. DOUTORADO/USP - Economia Aplicada/MATERIAS/Eco II - Daniel/Desafio Eco II - Pe de Meia/Github/pedemeia3/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="157" documentId="8_{F1CD36D2-19BE-47EB-AE65-13017DD7740D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{986DBBE4-0BAB-4DAF-8187-06135BE9A01D}"/>
+  <xr:revisionPtr revIDLastSave="159" documentId="8_{F1CD36D2-19BE-47EB-AE65-13017DD7740D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A771D721-A488-4C0A-A884-AAB03392664F}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{3F24F635-5B38-4FE0-8A30-7E7C7EEBC13B}"/>
   </bookViews>
@@ -124,7 +124,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1260" uniqueCount="355">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1023" uniqueCount="307">
   <si>
     <t>Coluna</t>
   </si>
@@ -693,310 +693,166 @@
     <t>Qualquer ano e trimestres</t>
   </si>
   <si>
-    <t>Pais</t>
-  </si>
-  <si>
     <t>País de origem dos dados (Brasil).</t>
   </si>
   <si>
     <t>Identificação e Controle</t>
   </si>
   <si>
-    <t>S01001Casa</t>
-  </si>
-  <si>
     <t>Proporção de domicílios em casas.</t>
   </si>
   <si>
-    <t>S01001Apartamento</t>
-  </si>
-  <si>
     <t>Proporção de domicílios em apartamentos.</t>
   </si>
   <si>
-    <t>S01001Habitação.em.casa.de.cômodos..cortiço.ou.cabeça.de.porco</t>
-  </si>
-  <si>
     <t>Proporção de habitações em condições precárias (como cortiços).</t>
   </si>
   <si>
-    <t>S01002Alvenaria.com.revestimento..taipa.com.revestimento</t>
-  </si>
-  <si>
     <t>Proporção de casas com paredes de alvenaria com revestimento.</t>
   </si>
   <si>
-    <t>S01002Alvenaria.sem.revestimento</t>
-  </si>
-  <si>
     <t>Proporção de casas de alvenaria sem revestimento.</t>
   </si>
   <si>
-    <t>S01002Taipa.sem.revestimento</t>
-  </si>
-  <si>
     <t>Proporção de casas de taipa sem revestimento.</t>
   </si>
   <si>
-    <t>S01002Madeira.apropriada.para.construção..aparelhada.</t>
-  </si>
-  <si>
     <t>Proporção de casas feitas de madeira apropriada para construção.</t>
   </si>
   <si>
-    <t>S01002Madeira.aproveitada</t>
-  </si>
-  <si>
     <t>Proporção de casas feitas com madeira reutilizada.</t>
   </si>
   <si>
-    <t>S01002Outro.material</t>
-  </si>
-  <si>
     <t>Proporção de casas feitas com outros materiais.</t>
   </si>
   <si>
-    <t>S01003Telha.sem.laje.de.concreto</t>
-  </si>
-  <si>
     <t>Proporção de telhados sem laje de concreto.</t>
   </si>
   <si>
-    <t>S01003Telha.com.laje.de.concreto</t>
-  </si>
-  <si>
     <t>Proporção de telhados com laje de concreto.</t>
   </si>
   <si>
-    <t>S01003Somente.laje.de.concreto</t>
-  </si>
-  <si>
     <t>Proporção de coberturas com apenas laje de concreto.</t>
   </si>
   <si>
-    <t>S01003Madeira.apropriada.para.construção</t>
-  </si>
-  <si>
     <t>Proporção de coberturas de madeira apropriada para construção.</t>
   </si>
   <si>
-    <t>S01003Zinco.alumínio.ou.chapa.metálica</t>
-  </si>
-  <si>
     <t>Proporção de coberturas com zinco, alumínio ou chapa metálica.</t>
   </si>
   <si>
-    <t>S01003Outro.material</t>
-  </si>
-  <si>
     <t>Proporção de coberturas com outros materiais.</t>
   </si>
   <si>
-    <t>S01004Cerâmica..lajota.ou.pedra</t>
-  </si>
-  <si>
     <t>Proporção de pisos de cerâmica, lajota ou pedra.</t>
   </si>
   <si>
-    <t>S01004Madeira.apropriada.para.construção</t>
-  </si>
-  <si>
     <t>Proporção de pisos de madeira apropriada para construção.</t>
   </si>
   <si>
-    <t>S01004Cimento</t>
-  </si>
-  <si>
     <t>Proporção de pisos de cimento.</t>
   </si>
   <si>
-    <t>S01004Terra</t>
-  </si>
-  <si>
     <t>Proporção de pisos de terra.</t>
   </si>
   <si>
-    <t>S01004Outro.material...especifique.</t>
-  </si>
-  <si>
     <t>Proporção de pisos de outros materiais especificados.</t>
   </si>
   <si>
-    <t>S01005</t>
-  </si>
-  <si>
     <t>Média de pessoas por domicílio.</t>
   </si>
   <si>
-    <t>S01006</t>
-  </si>
-  <si>
     <t>Número médio de cômodos por domicílio.</t>
   </si>
   <si>
-    <t>S01010Canalizada.em.pelo.menos.um.cômodo</t>
-  </si>
-  <si>
     <t>Proporção de domicílios com água canalizada em pelo menos um cômodo.</t>
   </si>
   <si>
     <t>Abastecimento de Água</t>
   </si>
   <si>
-    <t>S01010Canalizada.só.na.propriedade.ou.terreno</t>
-  </si>
-  <si>
     <t>Proporção de domicílios com água canalizada apenas na propriedade.</t>
   </si>
   <si>
-    <t>S01010Não.canalizada</t>
-  </si>
-  <si>
     <t>Proporção de domicílios sem água canalizada.</t>
   </si>
   <si>
-    <t>S01013Coletado.diretamente.por.serviço.de.limpeza</t>
-  </si>
-  <si>
     <t>Proporção de resíduos coletados por serviço de limpeza.</t>
   </si>
   <si>
     <t>Coleta de Lixo</t>
   </si>
   <si>
-    <t>S01013Coletado.em.caçamba.de.serviço.de.limpeza</t>
-  </si>
-  <si>
     <t>Proporção de resíduos coletados em caçambas de limpeza.</t>
   </si>
   <si>
-    <t>S01013Queimado..na.propriedade.</t>
-  </si>
-  <si>
     <t>Proporção de resíduos queimados na propriedade.</t>
   </si>
   <si>
-    <t>S01013Enterrado..na.propriedade.</t>
-  </si>
-  <si>
     <t>Proporção de resíduos enterrados na propriedade.</t>
   </si>
   <si>
-    <t>S01013Jogado.em.terreno.baldio.ou.logradouro</t>
-  </si>
-  <si>
     <t>Proporção de resíduos jogados em terrenos baldios.</t>
   </si>
   <si>
-    <t>S01013Outro.destino...especifique.</t>
-  </si>
-  <si>
     <t>Proporção de resíduos com outros destinos especificados.</t>
   </si>
   <si>
-    <t>S010141Sim</t>
-  </si>
-  <si>
     <t>Proporção de domicílios com esgoto canalizado.</t>
   </si>
   <si>
     <t>Saneamento</t>
   </si>
   <si>
-    <t>S010141Não</t>
-  </si>
-  <si>
     <t>Proporção de domicílios sem esgoto canalizado.</t>
   </si>
   <si>
-    <t>S01024Sim</t>
-  </si>
-  <si>
     <t>Proporção de domicílios com coleta de lixo.</t>
   </si>
   <si>
-    <t>S01024Não</t>
-  </si>
-  <si>
     <t>Proporção de domicílios sem coleta de lixo.</t>
   </si>
   <si>
-    <t>S01028Sim</t>
-  </si>
-  <si>
     <t>Proporção de domicílios com abastecimento de água.</t>
   </si>
   <si>
-    <t>S01028Não</t>
-  </si>
-  <si>
     <t>Proporção de domicílios sem abastecimento de água.</t>
   </si>
   <si>
-    <t>S010311Sim</t>
-  </si>
-  <si>
     <t>Proporção de domicílios com acesso a eletricidade.</t>
   </si>
   <si>
     <t>Eletricidade</t>
   </si>
   <si>
-    <t>S010311Não</t>
-  </si>
-  <si>
     <t>Proporção de domicílios sem acesso a eletricidade.</t>
   </si>
   <si>
-    <t>S010312Sim</t>
-  </si>
-  <si>
     <t>Proporção de domicílios com internet.</t>
   </si>
   <si>
     <t>Conectividade</t>
   </si>
   <si>
-    <t>S010312Não</t>
-  </si>
-  <si>
     <t>Proporção de domicílios sem internet.</t>
   </si>
   <si>
-    <t>se1 a se44</t>
-  </si>
-  <si>
     <t>Erros padrão das estimativas das variáveis correspondentes.</t>
   </si>
   <si>
     <t>Erro Padrão</t>
   </si>
   <si>
-    <t>cv.S01001Casa a cv.S010312Não</t>
-  </si>
-  <si>
     <t>Coeficiente de variação para cada variável, indicando a variabilidade relativa das estimativas.</t>
   </si>
   <si>
     <t>Variabilidade</t>
   </si>
   <si>
-    <t>GR</t>
-  </si>
-  <si>
     <t>Grande Região (Norte, Nordeste, Sudeste, Sul, Centro-Oeste) para a qual os dados são agregados.</t>
   </si>
   <si>
     <t>Região</t>
-  </si>
-  <si>
-    <t>descritiva_pnad_Mtl.R</t>
-  </si>
-  <si>
-    <t>M</t>
-  </si>
-  <si>
-    <t>descritiva_cadunico_Mtl.R</t>
   </si>
   <si>
     <t>UPA</t>
@@ -1255,7 +1111,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1316,14 +1172,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -1738,8 +1592,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{247AA1CF-A420-4D91-B350-1F036DB135E9}">
   <dimension ref="A1:H203"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="C89" sqref="C89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1757,7 +1611,7 @@
       <c r="A1" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="B1" s="24" t="s">
+      <c r="B1" s="23" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="3" t="s">
@@ -1775,7 +1629,7 @@
       <c r="G1" s="6" t="s">
         <v>127</v>
       </c>
-      <c r="H1" s="23" t="s">
+      <c r="H1" s="22" t="s">
         <v>3</v>
       </c>
     </row>
@@ -3983,17 +3837,15 @@
       </c>
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A86" s="22">
+      <c r="A86">
         <v>1</v>
       </c>
-      <c r="B86" s="9" t="s">
+      <c r="B86" s="9"/>
+      <c r="C86" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="C86" s="1" t="s">
+      <c r="D86" s="1" t="s">
         <v>190</v>
-      </c>
-      <c r="D86" s="1" t="s">
-        <v>191</v>
       </c>
       <c r="E86" s="8" t="str">
         <f t="shared" si="0"/>
@@ -4002,22 +3854,14 @@
       <c r="F86" s="9" t="s">
         <v>186</v>
       </c>
-      <c r="G86" s="7" t="s">
-        <v>288</v>
-      </c>
-      <c r="H86" s="7" t="s">
-        <v>289</v>
-      </c>
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A87" s="22">
+      <c r="A87">
         <v>2</v>
       </c>
-      <c r="B87" s="9" t="s">
-        <v>192</v>
-      </c>
+      <c r="B87" s="9"/>
       <c r="C87" s="1" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D87" s="1" t="s">
         <v>161</v>
@@ -4029,22 +3873,14 @@
       <c r="F87" s="9" t="s">
         <v>186</v>
       </c>
-      <c r="G87" s="7" t="s">
-        <v>288</v>
-      </c>
-      <c r="H87" s="7" t="s">
-        <v>289</v>
-      </c>
     </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A88" s="22">
+      <c r="A88">
         <v>3</v>
       </c>
-      <c r="B88" s="9" t="s">
-        <v>194</v>
-      </c>
+      <c r="B88" s="9"/>
       <c r="C88" s="1" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="D88" s="1" t="s">
         <v>161</v>
@@ -4056,22 +3892,14 @@
       <c r="F88" s="9" t="s">
         <v>186</v>
       </c>
-      <c r="G88" s="7" t="s">
-        <v>288</v>
-      </c>
-      <c r="H88" s="7" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="89" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A89" s="22">
-        <v>4</v>
-      </c>
-      <c r="B89" s="9" t="s">
-        <v>196</v>
-      </c>
+    </row>
+    <row r="89" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A89">
+        <v>4</v>
+      </c>
+      <c r="B89" s="9"/>
       <c r="C89" s="1" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="D89" s="1" t="s">
         <v>161</v>
@@ -4083,22 +3911,14 @@
       <c r="F89" s="9" t="s">
         <v>186</v>
       </c>
-      <c r="G89" s="7" t="s">
-        <v>288</v>
-      </c>
-      <c r="H89" s="7" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="90" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A90" s="22">
+    </row>
+    <row r="90" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A90">
         <v>5</v>
       </c>
-      <c r="B90" s="9" t="s">
-        <v>198</v>
-      </c>
+      <c r="B90" s="9"/>
       <c r="C90" s="1" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="D90" s="1" t="s">
         <v>139</v>
@@ -4110,22 +3930,14 @@
       <c r="F90" s="9" t="s">
         <v>186</v>
       </c>
-      <c r="G90" s="7" t="s">
-        <v>288</v>
-      </c>
-      <c r="H90" s="7" t="s">
-        <v>289</v>
-      </c>
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A91" s="22">
+      <c r="A91">
         <v>6</v>
       </c>
-      <c r="B91" s="9" t="s">
-        <v>200</v>
-      </c>
+      <c r="B91" s="9"/>
       <c r="C91" s="1" t="s">
-        <v>201</v>
+        <v>195</v>
       </c>
       <c r="D91" s="1" t="s">
         <v>139</v>
@@ -4137,22 +3949,14 @@
       <c r="F91" s="9" t="s">
         <v>186</v>
       </c>
-      <c r="G91" s="7" t="s">
-        <v>288</v>
-      </c>
-      <c r="H91" s="7" t="s">
-        <v>289</v>
-      </c>
     </row>
     <row r="92" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A92" s="22">
+      <c r="A92">
         <v>7</v>
       </c>
-      <c r="B92" s="9" t="s">
-        <v>202</v>
-      </c>
+      <c r="B92" s="9"/>
       <c r="C92" s="1" t="s">
-        <v>203</v>
+        <v>196</v>
       </c>
       <c r="D92" s="1" t="s">
         <v>139</v>
@@ -4164,22 +3968,14 @@
       <c r="F92" s="9" t="s">
         <v>186</v>
       </c>
-      <c r="G92" s="7" t="s">
-        <v>288</v>
-      </c>
-      <c r="H92" s="7" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="93" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A93" s="22">
+    </row>
+    <row r="93" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A93">
         <v>8</v>
       </c>
-      <c r="B93" s="9" t="s">
-        <v>204</v>
-      </c>
+      <c r="B93" s="9"/>
       <c r="C93" s="1" t="s">
-        <v>205</v>
+        <v>197</v>
       </c>
       <c r="D93" s="1" t="s">
         <v>139</v>
@@ -4191,22 +3987,14 @@
       <c r="F93" s="9" t="s">
         <v>186</v>
       </c>
-      <c r="G93" s="7" t="s">
-        <v>288</v>
-      </c>
-      <c r="H93" s="7" t="s">
-        <v>289</v>
-      </c>
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A94" s="22">
+      <c r="A94">
         <v>9</v>
       </c>
-      <c r="B94" s="9" t="s">
-        <v>206</v>
-      </c>
+      <c r="B94" s="9"/>
       <c r="C94" s="1" t="s">
-        <v>207</v>
+        <v>198</v>
       </c>
       <c r="D94" s="1" t="s">
         <v>139</v>
@@ -4218,22 +4006,14 @@
       <c r="F94" s="9" t="s">
         <v>186</v>
       </c>
-      <c r="G94" s="7" t="s">
-        <v>288</v>
-      </c>
-      <c r="H94" s="7" t="s">
-        <v>289</v>
-      </c>
     </row>
     <row r="95" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A95" s="22">
+      <c r="A95">
         <v>10</v>
       </c>
-      <c r="B95" s="9" t="s">
-        <v>208</v>
-      </c>
+      <c r="B95" s="9"/>
       <c r="C95" s="1" t="s">
-        <v>209</v>
+        <v>199</v>
       </c>
       <c r="D95" s="1" t="s">
         <v>139</v>
@@ -4245,22 +4025,14 @@
       <c r="F95" s="9" t="s">
         <v>186</v>
       </c>
-      <c r="G95" s="7" t="s">
-        <v>288</v>
-      </c>
-      <c r="H95" s="7" t="s">
-        <v>289</v>
-      </c>
     </row>
     <row r="96" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A96" s="22">
+      <c r="A96">
         <v>11</v>
       </c>
-      <c r="B96" s="9" t="s">
-        <v>210</v>
-      </c>
+      <c r="B96" s="9"/>
       <c r="C96" s="1" t="s">
-        <v>211</v>
+        <v>200</v>
       </c>
       <c r="D96" s="1" t="s">
         <v>139</v>
@@ -4272,22 +4044,14 @@
       <c r="F96" s="9" t="s">
         <v>186</v>
       </c>
-      <c r="G96" s="7" t="s">
-        <v>288</v>
-      </c>
-      <c r="H96" s="7" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A97" s="22">
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A97">
         <v>12</v>
       </c>
-      <c r="B97" s="9" t="s">
-        <v>212</v>
-      </c>
+      <c r="B97" s="9"/>
       <c r="C97" s="1" t="s">
-        <v>213</v>
+        <v>201</v>
       </c>
       <c r="D97" s="1" t="s">
         <v>139</v>
@@ -4299,22 +4063,14 @@
       <c r="F97" s="9" t="s">
         <v>186</v>
       </c>
-      <c r="G97" s="7" t="s">
-        <v>288</v>
-      </c>
-      <c r="H97" s="7" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A98" s="22">
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A98">
         <v>13</v>
       </c>
-      <c r="B98" s="9" t="s">
-        <v>214</v>
-      </c>
+      <c r="B98" s="9"/>
       <c r="C98" s="1" t="s">
-        <v>215</v>
+        <v>202</v>
       </c>
       <c r="D98" s="1" t="s">
         <v>139</v>
@@ -4326,22 +4082,14 @@
       <c r="F98" s="9" t="s">
         <v>186</v>
       </c>
-      <c r="G98" s="7" t="s">
-        <v>288</v>
-      </c>
-      <c r="H98" s="7" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A99" s="22">
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A99">
         <v>14</v>
       </c>
-      <c r="B99" s="9" t="s">
-        <v>216</v>
-      </c>
+      <c r="B99" s="9"/>
       <c r="C99" s="1" t="s">
-        <v>217</v>
+        <v>203</v>
       </c>
       <c r="D99" s="1" t="s">
         <v>139</v>
@@ -4353,22 +4101,14 @@
       <c r="F99" s="9" t="s">
         <v>186</v>
       </c>
-      <c r="G99" s="7" t="s">
-        <v>288</v>
-      </c>
-      <c r="H99" s="7" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A100" s="22">
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A100">
         <v>15</v>
       </c>
-      <c r="B100" s="9" t="s">
-        <v>218</v>
-      </c>
+      <c r="B100" s="9"/>
       <c r="C100" s="1" t="s">
-        <v>219</v>
+        <v>204</v>
       </c>
       <c r="D100" s="1" t="s">
         <v>139</v>
@@ -4380,22 +4120,14 @@
       <c r="F100" s="9" t="s">
         <v>186</v>
       </c>
-      <c r="G100" s="7" t="s">
-        <v>288</v>
-      </c>
-      <c r="H100" s="7" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A101" s="22">
+    </row>
+    <row r="101" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A101">
         <v>16</v>
       </c>
-      <c r="B101" s="9" t="s">
-        <v>220</v>
-      </c>
+      <c r="B101" s="9"/>
       <c r="C101" s="1" t="s">
-        <v>221</v>
+        <v>205</v>
       </c>
       <c r="D101" s="1" t="s">
         <v>139</v>
@@ -4407,22 +4139,14 @@
       <c r="F101" s="9" t="s">
         <v>186</v>
       </c>
-      <c r="G101" s="7" t="s">
-        <v>288</v>
-      </c>
-      <c r="H101" s="7" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A102" s="22">
+    </row>
+    <row r="102" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A102">
         <v>17</v>
       </c>
-      <c r="B102" s="9" t="s">
-        <v>222</v>
-      </c>
+      <c r="B102" s="9"/>
       <c r="C102" s="1" t="s">
-        <v>223</v>
+        <v>206</v>
       </c>
       <c r="D102" s="1" t="s">
         <v>139</v>
@@ -4434,22 +4158,14 @@
       <c r="F102" s="9" t="s">
         <v>186</v>
       </c>
-      <c r="G102" s="7" t="s">
-        <v>288</v>
-      </c>
-      <c r="H102" s="7" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A103" s="22">
+    </row>
+    <row r="103" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A103">
         <v>18</v>
       </c>
-      <c r="B103" s="9" t="s">
-        <v>224</v>
-      </c>
+      <c r="B103" s="9"/>
       <c r="C103" s="1" t="s">
-        <v>225</v>
+        <v>207</v>
       </c>
       <c r="D103" s="1" t="s">
         <v>139</v>
@@ -4461,22 +4177,14 @@
       <c r="F103" s="9" t="s">
         <v>186</v>
       </c>
-      <c r="G103" s="7" t="s">
-        <v>288</v>
-      </c>
-      <c r="H103" s="7" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A104" s="22">
+    </row>
+    <row r="104" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A104">
         <v>19</v>
       </c>
-      <c r="B104" s="9" t="s">
-        <v>226</v>
-      </c>
+      <c r="B104" s="9"/>
       <c r="C104" s="1" t="s">
-        <v>227</v>
+        <v>208</v>
       </c>
       <c r="D104" s="1" t="s">
         <v>139</v>
@@ -4488,22 +4196,14 @@
       <c r="F104" s="9" t="s">
         <v>186</v>
       </c>
-      <c r="G104" s="7" t="s">
-        <v>288</v>
-      </c>
-      <c r="H104" s="7" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="105" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A105" s="22">
+    </row>
+    <row r="105" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A105">
         <v>20</v>
       </c>
-      <c r="B105" s="9" t="s">
-        <v>228</v>
-      </c>
+      <c r="B105" s="9"/>
       <c r="C105" s="1" t="s">
-        <v>229</v>
+        <v>209</v>
       </c>
       <c r="D105" s="1" t="s">
         <v>139</v>
@@ -4515,22 +4215,14 @@
       <c r="F105" s="9" t="s">
         <v>186</v>
       </c>
-      <c r="G105" s="7" t="s">
-        <v>288</v>
-      </c>
-      <c r="H105" s="7" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="106" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A106" s="22">
+    </row>
+    <row r="106" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A106">
         <v>21</v>
       </c>
-      <c r="B106" s="9" t="s">
-        <v>230</v>
-      </c>
+      <c r="B106" s="9"/>
       <c r="C106" s="1" t="s">
-        <v>231</v>
+        <v>210</v>
       </c>
       <c r="D106" s="1" t="s">
         <v>139</v>
@@ -4542,22 +4234,14 @@
       <c r="F106" s="9" t="s">
         <v>186</v>
       </c>
-      <c r="G106" s="7" t="s">
-        <v>288</v>
-      </c>
-      <c r="H106" s="7" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="107" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A107" s="22">
+    </row>
+    <row r="107" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A107">
         <v>22</v>
       </c>
-      <c r="B107" s="9" t="s">
-        <v>232</v>
-      </c>
+      <c r="B107" s="9"/>
       <c r="C107" s="1" t="s">
-        <v>233</v>
+        <v>211</v>
       </c>
       <c r="D107" s="1" t="s">
         <v>140</v>
@@ -4569,22 +4253,14 @@
       <c r="F107" s="9" t="s">
         <v>186</v>
       </c>
-      <c r="G107" s="7" t="s">
-        <v>288</v>
-      </c>
-      <c r="H107" s="7" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="108" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A108" s="22">
+    </row>
+    <row r="108" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A108">
         <v>23</v>
       </c>
-      <c r="B108" s="9" t="s">
-        <v>234</v>
-      </c>
+      <c r="B108" s="9"/>
       <c r="C108" s="1" t="s">
-        <v>235</v>
+        <v>212</v>
       </c>
       <c r="D108" s="1" t="s">
         <v>139</v>
@@ -4596,25 +4272,17 @@
       <c r="F108" s="9" t="s">
         <v>186</v>
       </c>
-      <c r="G108" s="7" t="s">
-        <v>288</v>
-      </c>
-      <c r="H108" s="7" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="109" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A109" s="22">
+    </row>
+    <row r="109" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A109">
         <v>24</v>
       </c>
-      <c r="B109" s="9" t="s">
-        <v>236</v>
-      </c>
+      <c r="B109" s="9"/>
       <c r="C109" s="1" t="s">
-        <v>237</v>
+        <v>213</v>
       </c>
       <c r="D109" s="1" t="s">
-        <v>238</v>
+        <v>214</v>
       </c>
       <c r="E109" s="8" t="str">
         <f t="shared" si="0"/>
@@ -4623,25 +4291,17 @@
       <c r="F109" s="9" t="s">
         <v>186</v>
       </c>
-      <c r="G109" s="7" t="s">
-        <v>288</v>
-      </c>
-      <c r="H109" s="7" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="110" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A110" s="22">
+    </row>
+    <row r="110" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A110">
         <v>25</v>
       </c>
-      <c r="B110" s="9" t="s">
-        <v>239</v>
-      </c>
+      <c r="B110" s="9"/>
       <c r="C110" s="1" t="s">
-        <v>240</v>
+        <v>215</v>
       </c>
       <c r="D110" s="1" t="s">
-        <v>238</v>
+        <v>214</v>
       </c>
       <c r="E110" s="8" t="str">
         <f t="shared" si="0"/>
@@ -4650,25 +4310,17 @@
       <c r="F110" s="9" t="s">
         <v>186</v>
       </c>
-      <c r="G110" s="7" t="s">
-        <v>288</v>
-      </c>
-      <c r="H110" s="7" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="111" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A111" s="22">
+    </row>
+    <row r="111" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A111">
         <v>26</v>
       </c>
-      <c r="B111" s="9" t="s">
-        <v>241</v>
-      </c>
+      <c r="B111" s="9"/>
       <c r="C111" s="1" t="s">
-        <v>242</v>
+        <v>216</v>
       </c>
       <c r="D111" s="1" t="s">
-        <v>238</v>
+        <v>214</v>
       </c>
       <c r="E111" s="8" t="str">
         <f t="shared" si="0"/>
@@ -4677,25 +4329,17 @@
       <c r="F111" s="9" t="s">
         <v>186</v>
       </c>
-      <c r="G111" s="7" t="s">
-        <v>288</v>
-      </c>
-      <c r="H111" s="7" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="112" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A112" s="22">
+    </row>
+    <row r="112" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A112">
         <v>27</v>
       </c>
-      <c r="B112" s="9" t="s">
-        <v>243</v>
-      </c>
+      <c r="B112" s="9"/>
       <c r="C112" s="1" t="s">
-        <v>244</v>
+        <v>217</v>
       </c>
       <c r="D112" s="1" t="s">
-        <v>245</v>
+        <v>218</v>
       </c>
       <c r="E112" s="8" t="str">
         <f t="shared" si="0"/>
@@ -4704,25 +4348,17 @@
       <c r="F112" s="9" t="s">
         <v>186</v>
       </c>
-      <c r="G112" s="7" t="s">
-        <v>288</v>
-      </c>
-      <c r="H112" s="7" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="113" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A113" s="22">
+    </row>
+    <row r="113" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A113">
         <v>28</v>
       </c>
-      <c r="B113" s="9" t="s">
-        <v>246</v>
-      </c>
+      <c r="B113" s="9"/>
       <c r="C113" s="1" t="s">
-        <v>247</v>
+        <v>219</v>
       </c>
       <c r="D113" s="1" t="s">
-        <v>245</v>
+        <v>218</v>
       </c>
       <c r="E113" s="8" t="str">
         <f t="shared" si="0"/>
@@ -4731,25 +4367,17 @@
       <c r="F113" s="9" t="s">
         <v>186</v>
       </c>
-      <c r="G113" s="7" t="s">
-        <v>288</v>
-      </c>
-      <c r="H113" s="7" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="114" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A114" s="22">
+    </row>
+    <row r="114" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A114">
         <v>29</v>
       </c>
-      <c r="B114" s="9" t="s">
-        <v>248</v>
-      </c>
+      <c r="B114" s="9"/>
       <c r="C114" s="1" t="s">
-        <v>249</v>
+        <v>220</v>
       </c>
       <c r="D114" s="1" t="s">
-        <v>245</v>
+        <v>218</v>
       </c>
       <c r="E114" s="8" t="str">
         <f t="shared" si="0"/>
@@ -4758,25 +4386,17 @@
       <c r="F114" s="9" t="s">
         <v>186</v>
       </c>
-      <c r="G114" s="7" t="s">
-        <v>288</v>
-      </c>
-      <c r="H114" s="7" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="115" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A115" s="22">
+    </row>
+    <row r="115" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A115">
         <v>30</v>
       </c>
-      <c r="B115" s="9" t="s">
-        <v>250</v>
-      </c>
+      <c r="B115" s="9"/>
       <c r="C115" s="1" t="s">
-        <v>251</v>
+        <v>221</v>
       </c>
       <c r="D115" s="1" t="s">
-        <v>245</v>
+        <v>218</v>
       </c>
       <c r="E115" s="8" t="str">
         <f t="shared" si="0"/>
@@ -4785,25 +4405,17 @@
       <c r="F115" s="9" t="s">
         <v>186</v>
       </c>
-      <c r="G115" s="7" t="s">
-        <v>288</v>
-      </c>
-      <c r="H115" s="7" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="116" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A116" s="22">
+    </row>
+    <row r="116" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A116">
         <v>31</v>
       </c>
-      <c r="B116" s="9" t="s">
-        <v>252</v>
-      </c>
+      <c r="B116" s="9"/>
       <c r="C116" s="1" t="s">
-        <v>253</v>
+        <v>222</v>
       </c>
       <c r="D116" s="1" t="s">
-        <v>245</v>
+        <v>218</v>
       </c>
       <c r="E116" s="8" t="str">
         <f t="shared" si="0"/>
@@ -4812,25 +4424,17 @@
       <c r="F116" s="9" t="s">
         <v>186</v>
       </c>
-      <c r="G116" s="7" t="s">
-        <v>288</v>
-      </c>
-      <c r="H116" s="7" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="117" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A117" s="22">
+    </row>
+    <row r="117" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A117">
         <v>32</v>
       </c>
-      <c r="B117" s="9" t="s">
-        <v>254</v>
-      </c>
+      <c r="B117" s="9"/>
       <c r="C117" s="1" t="s">
-        <v>255</v>
+        <v>223</v>
       </c>
       <c r="D117" s="1" t="s">
-        <v>245</v>
+        <v>218</v>
       </c>
       <c r="E117" s="8" t="str">
         <f t="shared" si="0"/>
@@ -4839,25 +4443,17 @@
       <c r="F117" s="9" t="s">
         <v>186</v>
       </c>
-      <c r="G117" s="7" t="s">
-        <v>288</v>
-      </c>
-      <c r="H117" s="7" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="118" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A118" s="22">
+    </row>
+    <row r="118" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A118">
         <v>33</v>
       </c>
-      <c r="B118" s="9" t="s">
-        <v>256</v>
-      </c>
+      <c r="B118" s="9"/>
       <c r="C118" s="1" t="s">
-        <v>257</v>
+        <v>224</v>
       </c>
       <c r="D118" s="1" t="s">
-        <v>258</v>
+        <v>225</v>
       </c>
       <c r="E118" s="8" t="str">
         <f t="shared" si="0"/>
@@ -4866,25 +4462,17 @@
       <c r="F118" s="9" t="s">
         <v>186</v>
       </c>
-      <c r="G118" s="7" t="s">
-        <v>288</v>
-      </c>
-      <c r="H118" s="7" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="119" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A119" s="22">
+    </row>
+    <row r="119" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A119">
         <v>34</v>
       </c>
-      <c r="B119" s="9" t="s">
-        <v>259</v>
-      </c>
+      <c r="B119" s="9"/>
       <c r="C119" s="1" t="s">
-        <v>260</v>
+        <v>226</v>
       </c>
       <c r="D119" s="1" t="s">
-        <v>258</v>
+        <v>225</v>
       </c>
       <c r="E119" s="8" t="str">
         <f t="shared" si="0"/>
@@ -4893,25 +4481,17 @@
       <c r="F119" s="9" t="s">
         <v>186</v>
       </c>
-      <c r="G119" s="7" t="s">
-        <v>288</v>
-      </c>
-      <c r="H119" s="7" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="120" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A120" s="22">
+    </row>
+    <row r="120" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A120">
         <v>35</v>
       </c>
-      <c r="B120" s="9" t="s">
-        <v>261</v>
-      </c>
+      <c r="B120" s="9"/>
       <c r="C120" s="1" t="s">
-        <v>262</v>
+        <v>227</v>
       </c>
       <c r="D120" s="1" t="s">
-        <v>245</v>
+        <v>218</v>
       </c>
       <c r="E120" s="8" t="str">
         <f t="shared" si="0"/>
@@ -4920,25 +4500,17 @@
       <c r="F120" s="9" t="s">
         <v>186</v>
       </c>
-      <c r="G120" s="7" t="s">
-        <v>288</v>
-      </c>
-      <c r="H120" s="7" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="121" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A121" s="22">
+    </row>
+    <row r="121" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A121">
         <v>36</v>
       </c>
-      <c r="B121" s="9" t="s">
-        <v>263</v>
-      </c>
+      <c r="B121" s="9"/>
       <c r="C121" s="1" t="s">
-        <v>264</v>
+        <v>228</v>
       </c>
       <c r="D121" s="1" t="s">
-        <v>245</v>
+        <v>218</v>
       </c>
       <c r="E121" s="8" t="str">
         <f t="shared" si="0"/>
@@ -4947,25 +4519,17 @@
       <c r="F121" s="9" t="s">
         <v>186</v>
       </c>
-      <c r="G121" s="7" t="s">
-        <v>288</v>
-      </c>
-      <c r="H121" s="7" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="122" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A122" s="22">
+    </row>
+    <row r="122" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A122">
         <v>37</v>
       </c>
-      <c r="B122" s="9" t="s">
-        <v>265</v>
-      </c>
+      <c r="B122" s="9"/>
       <c r="C122" s="1" t="s">
-        <v>266</v>
+        <v>229</v>
       </c>
       <c r="D122" s="1" t="s">
-        <v>238</v>
+        <v>214</v>
       </c>
       <c r="E122" s="8" t="str">
         <f t="shared" si="0"/>
@@ -4974,25 +4538,17 @@
       <c r="F122" s="9" t="s">
         <v>186</v>
       </c>
-      <c r="G122" s="7" t="s">
-        <v>288</v>
-      </c>
-      <c r="H122" s="7" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="123" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A123" s="22">
+    </row>
+    <row r="123" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A123">
         <v>38</v>
       </c>
-      <c r="B123" s="9" t="s">
-        <v>267</v>
-      </c>
+      <c r="B123" s="9"/>
       <c r="C123" s="1" t="s">
-        <v>268</v>
+        <v>230</v>
       </c>
       <c r="D123" s="1" t="s">
-        <v>238</v>
+        <v>214</v>
       </c>
       <c r="E123" s="8" t="str">
         <f t="shared" si="0"/>
@@ -5001,25 +4557,17 @@
       <c r="F123" s="9" t="s">
         <v>186</v>
       </c>
-      <c r="G123" s="7" t="s">
-        <v>288</v>
-      </c>
-      <c r="H123" s="7" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="124" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A124" s="22">
+    </row>
+    <row r="124" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A124">
         <v>39</v>
       </c>
-      <c r="B124" s="9" t="s">
-        <v>269</v>
-      </c>
+      <c r="B124" s="9"/>
       <c r="C124" s="1" t="s">
-        <v>270</v>
+        <v>231</v>
       </c>
       <c r="D124" s="1" t="s">
-        <v>271</v>
+        <v>232</v>
       </c>
       <c r="E124" s="8" t="str">
         <f t="shared" si="0"/>
@@ -5028,25 +4576,17 @@
       <c r="F124" s="9" t="s">
         <v>186</v>
       </c>
-      <c r="G124" s="7" t="s">
-        <v>288</v>
-      </c>
-      <c r="H124" s="7" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="125" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A125" s="22">
+    </row>
+    <row r="125" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A125">
         <v>40</v>
       </c>
-      <c r="B125" s="9" t="s">
-        <v>272</v>
-      </c>
+      <c r="B125" s="9"/>
       <c r="C125" s="1" t="s">
-        <v>273</v>
+        <v>233</v>
       </c>
       <c r="D125" s="1" t="s">
-        <v>271</v>
+        <v>232</v>
       </c>
       <c r="E125" s="8" t="str">
         <f t="shared" si="0"/>
@@ -5055,25 +4595,17 @@
       <c r="F125" s="9" t="s">
         <v>186</v>
       </c>
-      <c r="G125" s="7" t="s">
-        <v>288</v>
-      </c>
-      <c r="H125" s="7" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="126" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A126" s="22">
+    </row>
+    <row r="126" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A126">
         <v>41</v>
       </c>
-      <c r="B126" s="9" t="s">
-        <v>274</v>
-      </c>
+      <c r="B126" s="9"/>
       <c r="C126" s="1" t="s">
-        <v>275</v>
+        <v>234</v>
       </c>
       <c r="D126" s="1" t="s">
-        <v>276</v>
+        <v>235</v>
       </c>
       <c r="E126" s="8" t="str">
         <f t="shared" si="0"/>
@@ -5082,25 +4614,17 @@
       <c r="F126" s="9" t="s">
         <v>186</v>
       </c>
-      <c r="G126" s="7" t="s">
-        <v>288</v>
-      </c>
-      <c r="H126" s="7" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="127" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A127" s="22">
+    </row>
+    <row r="127" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A127">
         <v>42</v>
       </c>
-      <c r="B127" s="9" t="s">
-        <v>277</v>
-      </c>
+      <c r="B127" s="9"/>
       <c r="C127" s="1" t="s">
-        <v>278</v>
+        <v>236</v>
       </c>
       <c r="D127" s="1" t="s">
-        <v>276</v>
+        <v>235</v>
       </c>
       <c r="E127" s="8" t="str">
         <f t="shared" si="0"/>
@@ -5109,25 +4633,17 @@
       <c r="F127" s="9" t="s">
         <v>186</v>
       </c>
-      <c r="G127" s="7" t="s">
-        <v>288</v>
-      </c>
-      <c r="H127" s="7" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="128" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A128" s="22">
+    </row>
+    <row r="128" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A128">
         <v>43</v>
       </c>
-      <c r="B128" s="9" t="s">
-        <v>279</v>
-      </c>
+      <c r="B128" s="9"/>
       <c r="C128" s="1" t="s">
-        <v>280</v>
+        <v>237</v>
       </c>
       <c r="D128" s="1" t="s">
-        <v>281</v>
+        <v>238</v>
       </c>
       <c r="E128" s="8" t="str">
         <f t="shared" si="0"/>
@@ -5136,25 +4652,17 @@
       <c r="F128" s="9" t="s">
         <v>186</v>
       </c>
-      <c r="G128" s="7" t="s">
-        <v>288</v>
-      </c>
-      <c r="H128" s="7" t="s">
-        <v>289</v>
-      </c>
     </row>
     <row r="129" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A129" s="22">
+      <c r="A129">
         <v>44</v>
       </c>
-      <c r="B129" s="9" t="s">
-        <v>282</v>
-      </c>
+      <c r="B129" s="9"/>
       <c r="C129" s="1" t="s">
-        <v>283</v>
+        <v>239</v>
       </c>
       <c r="D129" s="1" t="s">
-        <v>284</v>
+        <v>240</v>
       </c>
       <c r="E129" s="8" t="str">
         <f t="shared" si="0"/>
@@ -5163,25 +4671,17 @@
       <c r="F129" s="9" t="s">
         <v>186</v>
       </c>
-      <c r="G129" s="7" t="s">
-        <v>288</v>
-      </c>
-      <c r="H129" s="7" t="s">
-        <v>289</v>
-      </c>
     </row>
     <row r="130" spans="1:8" s="10" customFormat="1" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A130" s="25">
+      <c r="A130" s="10">
         <v>45</v>
       </c>
-      <c r="B130" s="16" t="s">
-        <v>285</v>
-      </c>
+      <c r="B130" s="16"/>
       <c r="C130" s="11" t="s">
-        <v>286</v>
+        <v>241</v>
       </c>
       <c r="D130" s="11" t="s">
-        <v>287</v>
+        <v>242</v>
       </c>
       <c r="E130" s="20" t="str">
         <f t="shared" si="0"/>
@@ -5190,20 +4690,14 @@
       <c r="F130" s="16" t="s">
         <v>186</v>
       </c>
-      <c r="G130" s="12" t="s">
-        <v>288</v>
-      </c>
-      <c r="H130" s="12" t="s">
-        <v>289</v>
-      </c>
+      <c r="G130" s="12"/>
+      <c r="H130" s="12"/>
     </row>
     <row r="131" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A131" s="22">
+      <c r="A131">
         <v>1</v>
       </c>
-      <c r="B131" s="1" t="s">
-        <v>5</v>
-      </c>
+      <c r="B131" s="1"/>
       <c r="C131" s="1" t="s">
         <v>6</v>
       </c>
@@ -5216,20 +4710,12 @@
       <c r="F131" s="9" t="s">
         <v>129</v>
       </c>
-      <c r="G131" s="7" t="s">
-        <v>290</v>
-      </c>
-      <c r="H131" s="7" t="s">
-        <v>289</v>
-      </c>
     </row>
     <row r="132" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A132" s="22">
+      <c r="A132">
         <v>2</v>
       </c>
-      <c r="B132" s="1" t="s">
-        <v>7</v>
-      </c>
+      <c r="B132" s="1"/>
       <c r="C132" s="1" t="s">
         <v>8</v>
       </c>
@@ -5242,20 +4728,12 @@
       <c r="F132" s="9" t="s">
         <v>129</v>
       </c>
-      <c r="G132" s="7" t="s">
-        <v>290</v>
-      </c>
-      <c r="H132" s="7" t="s">
-        <v>289</v>
-      </c>
     </row>
     <row r="133" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A133" s="22">
+      <c r="A133">
         <v>3</v>
       </c>
-      <c r="B133" s="1" t="s">
-        <v>9</v>
-      </c>
+      <c r="B133" s="1"/>
       <c r="C133" s="1" t="s">
         <v>10</v>
       </c>
@@ -5268,20 +4746,12 @@
       <c r="F133" s="9" t="s">
         <v>129</v>
       </c>
-      <c r="G133" s="7" t="s">
-        <v>290</v>
-      </c>
-      <c r="H133" s="7" t="s">
-        <v>289</v>
-      </c>
     </row>
     <row r="134" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A134" s="22">
-        <v>4</v>
-      </c>
-      <c r="B134" s="1" t="s">
-        <v>11</v>
-      </c>
+      <c r="A134">
+        <v>4</v>
+      </c>
+      <c r="B134" s="1"/>
       <c r="C134" s="1" t="s">
         <v>12</v>
       </c>
@@ -5294,20 +4764,12 @@
       <c r="F134" s="9" t="s">
         <v>129</v>
       </c>
-      <c r="G134" s="7" t="s">
-        <v>290</v>
-      </c>
-      <c r="H134" s="7" t="s">
-        <v>289</v>
-      </c>
     </row>
     <row r="135" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A135" s="22">
+      <c r="A135">
         <v>5</v>
       </c>
-      <c r="B135" s="1" t="s">
-        <v>67</v>
-      </c>
+      <c r="B135" s="1"/>
       <c r="C135" s="1" t="s">
         <v>68</v>
       </c>
@@ -5320,20 +4782,12 @@
       <c r="F135" s="9" t="s">
         <v>129</v>
       </c>
-      <c r="G135" s="7" t="s">
-        <v>290</v>
-      </c>
-      <c r="H135" s="7" t="s">
-        <v>289</v>
-      </c>
     </row>
     <row r="136" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A136" s="22">
+      <c r="A136">
         <v>6</v>
       </c>
-      <c r="B136" s="1" t="s">
-        <v>69</v>
-      </c>
+      <c r="B136" s="1"/>
       <c r="C136" s="1" t="s">
         <v>70</v>
       </c>
@@ -5346,20 +4800,12 @@
       <c r="F136" s="9" t="s">
         <v>129</v>
       </c>
-      <c r="G136" s="7" t="s">
-        <v>290</v>
-      </c>
-      <c r="H136" s="7" t="s">
-        <v>289</v>
-      </c>
     </row>
     <row r="137" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A137" s="22">
+      <c r="A137">
         <v>7</v>
       </c>
-      <c r="B137" s="1" t="s">
-        <v>71</v>
-      </c>
+      <c r="B137" s="1"/>
       <c r="C137" s="1" t="s">
         <v>72</v>
       </c>
@@ -5372,20 +4818,12 @@
       <c r="F137" s="9" t="s">
         <v>129</v>
       </c>
-      <c r="G137" s="7" t="s">
-        <v>290</v>
-      </c>
-      <c r="H137" s="7" t="s">
-        <v>289</v>
-      </c>
     </row>
     <row r="138" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A138" s="22">
+      <c r="A138">
         <v>8</v>
       </c>
-      <c r="B138" s="1" t="s">
-        <v>73</v>
-      </c>
+      <c r="B138" s="1"/>
       <c r="C138" s="1" t="s">
         <v>74</v>
       </c>
@@ -5398,20 +4836,12 @@
       <c r="F138" s="9" t="s">
         <v>129</v>
       </c>
-      <c r="G138" s="7" t="s">
-        <v>290</v>
-      </c>
-      <c r="H138" s="7" t="s">
-        <v>289</v>
-      </c>
     </row>
     <row r="139" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A139" s="22">
+      <c r="A139">
         <v>9</v>
       </c>
-      <c r="B139" s="1" t="s">
-        <v>75</v>
-      </c>
+      <c r="B139" s="1"/>
       <c r="C139" s="1" t="s">
         <v>76</v>
       </c>
@@ -5424,20 +4854,12 @@
       <c r="F139" s="9" t="s">
         <v>129</v>
       </c>
-      <c r="G139" s="7" t="s">
-        <v>290</v>
-      </c>
-      <c r="H139" s="7" t="s">
-        <v>289</v>
-      </c>
     </row>
     <row r="140" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A140" s="22">
+      <c r="A140">
         <v>10</v>
       </c>
-      <c r="B140" s="1" t="s">
-        <v>77</v>
-      </c>
+      <c r="B140" s="1"/>
       <c r="C140" s="1" t="s">
         <v>78</v>
       </c>
@@ -5450,20 +4872,12 @@
       <c r="F140" s="9" t="s">
         <v>129</v>
       </c>
-      <c r="G140" s="7" t="s">
-        <v>290</v>
-      </c>
-      <c r="H140" s="7" t="s">
-        <v>289</v>
-      </c>
     </row>
     <row r="141" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A141" s="22">
+      <c r="A141">
         <v>11</v>
       </c>
-      <c r="B141" s="1" t="s">
-        <v>79</v>
-      </c>
+      <c r="B141" s="1"/>
       <c r="C141" s="1" t="s">
         <v>80</v>
       </c>
@@ -5476,20 +4890,12 @@
       <c r="F141" s="9" t="s">
         <v>129</v>
       </c>
-      <c r="G141" s="7" t="s">
-        <v>290</v>
-      </c>
-      <c r="H141" s="7" t="s">
-        <v>289</v>
-      </c>
     </row>
     <row r="142" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A142" s="22">
+      <c r="A142">
         <v>12</v>
       </c>
-      <c r="B142" s="1" t="s">
-        <v>81</v>
-      </c>
+      <c r="B142" s="1"/>
       <c r="C142" s="1" t="s">
         <v>82</v>
       </c>
@@ -5502,20 +4908,12 @@
       <c r="F142" s="9" t="s">
         <v>129</v>
       </c>
-      <c r="G142" s="7" t="s">
-        <v>290</v>
-      </c>
-      <c r="H142" s="7" t="s">
-        <v>289</v>
-      </c>
     </row>
     <row r="143" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A143" s="22">
+      <c r="A143">
         <v>13</v>
       </c>
-      <c r="B143" s="1" t="s">
-        <v>83</v>
-      </c>
+      <c r="B143" s="1"/>
       <c r="C143" s="1" t="s">
         <v>84</v>
       </c>
@@ -5528,20 +4926,12 @@
       <c r="F143" s="9" t="s">
         <v>129</v>
       </c>
-      <c r="G143" s="7" t="s">
-        <v>290</v>
-      </c>
-      <c r="H143" s="7" t="s">
-        <v>289</v>
-      </c>
     </row>
     <row r="144" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A144" s="22">
+      <c r="A144">
         <v>14</v>
       </c>
-      <c r="B144" s="1" t="s">
-        <v>85</v>
-      </c>
+      <c r="B144" s="1"/>
       <c r="C144" s="1" t="s">
         <v>86</v>
       </c>
@@ -5554,20 +4944,12 @@
       <c r="F144" s="9" t="s">
         <v>129</v>
       </c>
-      <c r="G144" s="7" t="s">
-        <v>290</v>
-      </c>
-      <c r="H144" s="7" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="145" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A145" s="22">
+    </row>
+    <row r="145" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A145">
         <v>15</v>
       </c>
-      <c r="B145" s="1" t="s">
-        <v>87</v>
-      </c>
+      <c r="B145" s="1"/>
       <c r="C145" s="1" t="s">
         <v>88</v>
       </c>
@@ -5580,20 +4962,12 @@
       <c r="F145" s="9" t="s">
         <v>129</v>
       </c>
-      <c r="G145" s="7" t="s">
-        <v>290</v>
-      </c>
-      <c r="H145" s="7" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="146" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A146" s="22">
+    </row>
+    <row r="146" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A146">
         <v>16</v>
       </c>
-      <c r="B146" s="1" t="s">
-        <v>89</v>
-      </c>
+      <c r="B146" s="1"/>
       <c r="C146" s="1" t="s">
         <v>90</v>
       </c>
@@ -5606,20 +4980,12 @@
       <c r="F146" s="9" t="s">
         <v>129</v>
       </c>
-      <c r="G146" s="7" t="s">
-        <v>290</v>
-      </c>
-      <c r="H146" s="7" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="147" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A147" s="22">
+    </row>
+    <row r="147" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A147">
         <v>17</v>
       </c>
-      <c r="B147" s="1" t="s">
-        <v>91</v>
-      </c>
+      <c r="B147" s="1"/>
       <c r="C147" s="1" t="s">
         <v>92</v>
       </c>
@@ -5632,20 +4998,12 @@
       <c r="F147" s="9" t="s">
         <v>129</v>
       </c>
-      <c r="G147" s="7" t="s">
-        <v>290</v>
-      </c>
-      <c r="H147" s="7" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="148" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A148" s="22">
+    </row>
+    <row r="148" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A148">
         <v>18</v>
       </c>
-      <c r="B148" s="1" t="s">
-        <v>93</v>
-      </c>
+      <c r="B148" s="1"/>
       <c r="C148" s="1" t="s">
         <v>94</v>
       </c>
@@ -5658,20 +5016,12 @@
       <c r="F148" s="9" t="s">
         <v>129</v>
       </c>
-      <c r="G148" s="7" t="s">
-        <v>290</v>
-      </c>
-      <c r="H148" s="7" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="149" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A149" s="22">
+    </row>
+    <row r="149" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A149">
         <v>19</v>
       </c>
-      <c r="B149" s="1" t="s">
-        <v>95</v>
-      </c>
+      <c r="B149" s="1"/>
       <c r="C149" s="1" t="s">
         <v>96</v>
       </c>
@@ -5684,20 +5034,12 @@
       <c r="F149" s="9" t="s">
         <v>129</v>
       </c>
-      <c r="G149" s="7" t="s">
-        <v>290</v>
-      </c>
-      <c r="H149" s="7" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="150" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A150" s="22">
+    </row>
+    <row r="150" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A150">
         <v>20</v>
       </c>
-      <c r="B150" s="1" t="s">
-        <v>97</v>
-      </c>
+      <c r="B150" s="1"/>
       <c r="C150" s="1" t="s">
         <v>98</v>
       </c>
@@ -5710,20 +5052,12 @@
       <c r="F150" s="9" t="s">
         <v>129</v>
       </c>
-      <c r="G150" s="7" t="s">
-        <v>290</v>
-      </c>
-      <c r="H150" s="7" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="151" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A151" s="22">
+    </row>
+    <row r="151" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A151">
         <v>21</v>
       </c>
-      <c r="B151" s="1" t="s">
-        <v>99</v>
-      </c>
+      <c r="B151" s="1"/>
       <c r="C151" s="1" t="s">
         <v>100</v>
       </c>
@@ -5736,20 +5070,12 @@
       <c r="F151" s="9" t="s">
         <v>129</v>
       </c>
-      <c r="G151" s="7" t="s">
-        <v>290</v>
-      </c>
-      <c r="H151" s="7" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="152" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A152" s="22">
+    </row>
+    <row r="152" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A152">
         <v>22</v>
       </c>
-      <c r="B152" s="1" t="s">
-        <v>101</v>
-      </c>
+      <c r="B152" s="1"/>
       <c r="C152" s="1" t="s">
         <v>102</v>
       </c>
@@ -5762,20 +5088,12 @@
       <c r="F152" s="9" t="s">
         <v>129</v>
       </c>
-      <c r="G152" s="7" t="s">
-        <v>290</v>
-      </c>
-      <c r="H152" s="7" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="153" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A153" s="22">
+    </row>
+    <row r="153" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A153">
         <v>23</v>
       </c>
-      <c r="B153" s="1" t="s">
-        <v>103</v>
-      </c>
+      <c r="B153" s="1"/>
       <c r="C153" s="1" t="s">
         <v>104</v>
       </c>
@@ -5788,20 +5106,12 @@
       <c r="F153" s="9" t="s">
         <v>129</v>
       </c>
-      <c r="G153" s="7" t="s">
-        <v>290</v>
-      </c>
-      <c r="H153" s="7" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="154" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A154" s="22">
+    </row>
+    <row r="154" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A154">
         <v>24</v>
       </c>
-      <c r="B154" s="1" t="s">
-        <v>105</v>
-      </c>
+      <c r="B154" s="1"/>
       <c r="C154" s="1" t="s">
         <v>106</v>
       </c>
@@ -5814,20 +5124,12 @@
       <c r="F154" s="9" t="s">
         <v>129</v>
       </c>
-      <c r="G154" s="7" t="s">
-        <v>290</v>
-      </c>
-      <c r="H154" s="7" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="155" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A155" s="22">
+    </row>
+    <row r="155" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A155">
         <v>25</v>
       </c>
-      <c r="B155" s="1" t="s">
-        <v>107</v>
-      </c>
+      <c r="B155" s="1"/>
       <c r="C155" s="1" t="s">
         <v>108</v>
       </c>
@@ -5840,20 +5142,12 @@
       <c r="F155" s="9" t="s">
         <v>129</v>
       </c>
-      <c r="G155" s="7" t="s">
-        <v>290</v>
-      </c>
-      <c r="H155" s="7" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="156" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A156" s="22">
+    </row>
+    <row r="156" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A156">
         <v>26</v>
       </c>
-      <c r="B156" s="1" t="s">
-        <v>109</v>
-      </c>
+      <c r="B156" s="1"/>
       <c r="C156" s="1" t="s">
         <v>110</v>
       </c>
@@ -5866,20 +5160,12 @@
       <c r="F156" s="9" t="s">
         <v>129</v>
       </c>
-      <c r="G156" s="7" t="s">
-        <v>290</v>
-      </c>
-      <c r="H156" s="7" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="157" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A157" s="22">
+    </row>
+    <row r="157" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A157">
         <v>27</v>
       </c>
-      <c r="B157" s="1" t="s">
-        <v>111</v>
-      </c>
+      <c r="B157" s="1"/>
       <c r="C157" s="1" t="s">
         <v>112</v>
       </c>
@@ -5892,20 +5178,12 @@
       <c r="F157" s="9" t="s">
         <v>129</v>
       </c>
-      <c r="G157" s="7" t="s">
-        <v>290</v>
-      </c>
-      <c r="H157" s="7" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="158" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A158" s="22">
+    </row>
+    <row r="158" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A158">
         <v>28</v>
       </c>
-      <c r="B158" s="1" t="s">
-        <v>113</v>
-      </c>
+      <c r="B158" s="1"/>
       <c r="C158" s="1" t="s">
         <v>114</v>
       </c>
@@ -5918,20 +5196,12 @@
       <c r="F158" s="9" t="s">
         <v>129</v>
       </c>
-      <c r="G158" s="7" t="s">
-        <v>290</v>
-      </c>
-      <c r="H158" s="7" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="159" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A159" s="22">
+    </row>
+    <row r="159" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A159">
         <v>29</v>
       </c>
-      <c r="B159" s="1" t="s">
-        <v>115</v>
-      </c>
+      <c r="B159" s="1"/>
       <c r="C159" s="1" t="s">
         <v>116</v>
       </c>
@@ -5944,20 +5214,12 @@
       <c r="F159" s="9" t="s">
         <v>129</v>
       </c>
-      <c r="G159" s="7" t="s">
-        <v>290</v>
-      </c>
-      <c r="H159" s="7" t="s">
-        <v>289</v>
-      </c>
-    </row>
-    <row r="160" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A160" s="22">
+    </row>
+    <row r="160" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A160">
         <v>30</v>
       </c>
-      <c r="B160" s="1" t="s">
-        <v>117</v>
-      </c>
+      <c r="B160" s="1"/>
       <c r="C160" s="1" t="s">
         <v>118</v>
       </c>
@@ -5970,20 +5232,12 @@
       <c r="F160" s="9" t="s">
         <v>129</v>
       </c>
-      <c r="G160" s="7" t="s">
-        <v>290</v>
-      </c>
-      <c r="H160" s="7" t="s">
-        <v>289</v>
-      </c>
     </row>
     <row r="161" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A161" s="22">
+      <c r="A161">
         <v>31</v>
       </c>
-      <c r="B161" s="1" t="s">
-        <v>119</v>
-      </c>
+      <c r="B161" s="1"/>
       <c r="C161" s="1" t="s">
         <v>120</v>
       </c>
@@ -5996,20 +5250,12 @@
       <c r="F161" s="9" t="s">
         <v>129</v>
       </c>
-      <c r="G161" s="7" t="s">
-        <v>290</v>
-      </c>
-      <c r="H161" s="7" t="s">
-        <v>289</v>
-      </c>
     </row>
     <row r="162" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A162" s="22">
+      <c r="A162">
         <v>32</v>
       </c>
-      <c r="B162" s="1" t="s">
-        <v>121</v>
-      </c>
+      <c r="B162" s="1"/>
       <c r="C162" s="1" t="s">
         <v>122</v>
       </c>
@@ -6022,20 +5268,12 @@
       <c r="F162" s="9" t="s">
         <v>129</v>
       </c>
-      <c r="G162" s="7" t="s">
-        <v>290</v>
-      </c>
-      <c r="H162" s="7" t="s">
-        <v>289</v>
-      </c>
     </row>
     <row r="163" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A163" s="22">
+      <c r="A163">
         <v>33</v>
       </c>
-      <c r="B163" s="1" t="s">
-        <v>123</v>
-      </c>
+      <c r="B163" s="1"/>
       <c r="C163" s="1" t="s">
         <v>124</v>
       </c>
@@ -6048,171 +5286,159 @@
       <c r="F163" s="9" t="s">
         <v>129</v>
       </c>
-      <c r="G163" s="7" t="s">
-        <v>290</v>
-      </c>
-      <c r="H163" s="7" t="s">
-        <v>289</v>
-      </c>
     </row>
     <row r="164" spans="1:8" s="10" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A164" s="25">
+      <c r="A164" s="10">
         <v>34</v>
       </c>
-      <c r="B164" s="11" t="s">
-        <v>65</v>
-      </c>
+      <c r="B164" s="11"/>
       <c r="C164" s="11" t="s">
         <v>66</v>
       </c>
       <c r="D164" s="11" t="s">
         <v>143</v>
       </c>
-      <c r="E164" s="26">
+      <c r="E164" s="24">
         <v>2017</v>
       </c>
       <c r="F164" s="16" t="s">
         <v>129</v>
       </c>
-      <c r="G164" s="12" t="s">
-        <v>290</v>
-      </c>
-      <c r="H164" s="12" t="s">
-        <v>289</v>
-      </c>
+      <c r="G164" s="12"/>
+      <c r="H164" s="12"/>
     </row>
     <row r="165" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A165" s="22">
+      <c r="A165">
         <v>1</v>
       </c>
       <c r="B165" s="1" t="s">
-        <v>291</v>
+        <v>243</v>
       </c>
       <c r="C165" s="1" t="s">
-        <v>292</v>
+        <v>244</v>
       </c>
       <c r="D165" s="1" t="s">
         <v>143</v>
       </c>
       <c r="E165" s="19" t="s">
-        <v>352</v>
+        <v>304</v>
       </c>
       <c r="F165" s="9" t="s">
         <v>186</v>
       </c>
       <c r="G165" s="7" t="s">
-        <v>353</v>
+        <v>305</v>
       </c>
       <c r="H165" s="7" t="s">
-        <v>354</v>
+        <v>306</v>
       </c>
     </row>
     <row r="166" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A166" s="22">
+      <c r="A166">
         <v>2</v>
       </c>
       <c r="B166" s="1" t="s">
-        <v>293</v>
+        <v>245</v>
       </c>
       <c r="C166" s="1" t="s">
-        <v>294</v>
+        <v>246</v>
       </c>
       <c r="D166" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E166" s="19" t="s">
-        <v>352</v>
+        <v>304</v>
       </c>
       <c r="F166" s="9" t="s">
         <v>186</v>
       </c>
       <c r="G166" s="7" t="s">
-        <v>353</v>
+        <v>305</v>
       </c>
       <c r="H166" s="7" t="s">
-        <v>354</v>
+        <v>306</v>
       </c>
     </row>
     <row r="167" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A167" s="22">
+      <c r="A167">
         <v>3</v>
       </c>
       <c r="B167" s="1" t="s">
-        <v>295</v>
+        <v>247</v>
       </c>
       <c r="C167" s="1" t="s">
-        <v>296</v>
+        <v>248</v>
       </c>
       <c r="D167" s="1" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="E167" s="19" t="s">
-        <v>352</v>
+        <v>304</v>
       </c>
       <c r="F167" s="9" t="s">
         <v>186</v>
       </c>
       <c r="G167" s="7" t="s">
-        <v>353</v>
+        <v>305</v>
       </c>
       <c r="H167" s="7" t="s">
-        <v>354</v>
+        <v>306</v>
       </c>
     </row>
     <row r="168" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A168" s="22">
+      <c r="A168">
         <v>4</v>
       </c>
       <c r="B168" s="1" t="s">
-        <v>297</v>
+        <v>249</v>
       </c>
       <c r="C168" s="1" t="s">
-        <v>298</v>
+        <v>250</v>
       </c>
       <c r="D168" s="1" t="s">
-        <v>299</v>
+        <v>251</v>
       </c>
       <c r="E168" s="19" t="s">
-        <v>352</v>
+        <v>304</v>
       </c>
       <c r="F168" s="9" t="s">
         <v>186</v>
       </c>
       <c r="G168" s="7" t="s">
-        <v>353</v>
+        <v>305</v>
       </c>
       <c r="H168" s="7" t="s">
-        <v>354</v>
+        <v>306</v>
       </c>
     </row>
     <row r="169" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A169" s="22">
+      <c r="A169">
         <v>5</v>
       </c>
       <c r="B169" s="1" t="s">
-        <v>300</v>
+        <v>252</v>
       </c>
       <c r="C169" s="1" t="s">
-        <v>301</v>
+        <v>253</v>
       </c>
       <c r="D169" s="1" t="s">
-        <v>299</v>
+        <v>251</v>
       </c>
       <c r="E169" s="19" t="s">
-        <v>352</v>
+        <v>304</v>
       </c>
       <c r="F169" s="9" t="s">
         <v>186</v>
       </c>
       <c r="G169" s="7" t="s">
-        <v>353</v>
+        <v>305</v>
       </c>
       <c r="H169" s="7" t="s">
-        <v>354</v>
+        <v>306</v>
       </c>
     </row>
     <row r="170" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A170" s="22">
+      <c r="A170">
         <v>6</v>
       </c>
       <c r="B170" s="1" t="s">
@@ -6225,72 +5451,72 @@
         <v>138</v>
       </c>
       <c r="E170" s="19" t="s">
-        <v>352</v>
+        <v>304</v>
       </c>
       <c r="F170" s="9" t="s">
         <v>186</v>
       </c>
       <c r="G170" s="7" t="s">
-        <v>353</v>
+        <v>305</v>
       </c>
       <c r="H170" s="7" t="s">
-        <v>354</v>
+        <v>306</v>
       </c>
     </row>
     <row r="171" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A171" s="22">
+      <c r="A171">
         <v>7</v>
       </c>
       <c r="B171" s="1" t="s">
-        <v>302</v>
+        <v>254</v>
       </c>
       <c r="C171" s="1" t="s">
-        <v>303</v>
+        <v>255</v>
       </c>
       <c r="D171" s="1" t="s">
         <v>138</v>
       </c>
       <c r="E171" s="19" t="s">
-        <v>352</v>
+        <v>304</v>
       </c>
       <c r="F171" s="9" t="s">
         <v>186</v>
       </c>
       <c r="G171" s="7" t="s">
-        <v>353</v>
+        <v>305</v>
       </c>
       <c r="H171" s="7" t="s">
-        <v>354</v>
+        <v>306</v>
       </c>
     </row>
     <row r="172" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A172" s="22">
+      <c r="A172">
         <v>8</v>
       </c>
       <c r="B172" s="1" t="s">
-        <v>304</v>
+        <v>256</v>
       </c>
       <c r="C172" s="1" t="s">
-        <v>305</v>
+        <v>257</v>
       </c>
       <c r="D172" s="1" t="s">
         <v>138</v>
       </c>
       <c r="E172" s="19" t="s">
-        <v>352</v>
+        <v>304</v>
       </c>
       <c r="F172" s="9" t="s">
         <v>186</v>
       </c>
       <c r="G172" s="7" t="s">
-        <v>353</v>
+        <v>305</v>
       </c>
       <c r="H172" s="7" t="s">
-        <v>354</v>
+        <v>306</v>
       </c>
     </row>
     <row r="173" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A173" s="22">
+      <c r="A173">
         <v>9</v>
       </c>
       <c r="B173" s="1" t="s">
@@ -6303,20 +5529,20 @@
         <v>154</v>
       </c>
       <c r="E173" s="19" t="s">
-        <v>352</v>
+        <v>304</v>
       </c>
       <c r="F173" s="9" t="s">
         <v>186</v>
       </c>
       <c r="G173" s="7" t="s">
-        <v>353</v>
+        <v>305</v>
       </c>
       <c r="H173" s="7" t="s">
-        <v>354</v>
+        <v>306</v>
       </c>
     </row>
     <row r="174" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A174" s="22">
+      <c r="A174">
         <v>10</v>
       </c>
       <c r="B174" s="1" t="s">
@@ -6329,20 +5555,20 @@
         <v>161</v>
       </c>
       <c r="E174" s="19" t="s">
-        <v>352</v>
+        <v>304</v>
       </c>
       <c r="F174" s="9" t="s">
         <v>186</v>
       </c>
       <c r="G174" s="7" t="s">
-        <v>353</v>
+        <v>305</v>
       </c>
       <c r="H174" s="7" t="s">
-        <v>354</v>
+        <v>306</v>
       </c>
     </row>
     <row r="175" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A175" s="22">
+      <c r="A175">
         <v>11</v>
       </c>
       <c r="B175" s="1" t="s">
@@ -6355,20 +5581,20 @@
         <v>140</v>
       </c>
       <c r="E175" s="19" t="s">
-        <v>352</v>
+        <v>304</v>
       </c>
       <c r="F175" s="9" t="s">
         <v>186</v>
       </c>
       <c r="G175" s="7" t="s">
-        <v>353</v>
+        <v>305</v>
       </c>
       <c r="H175" s="7" t="s">
-        <v>354</v>
+        <v>306</v>
       </c>
     </row>
     <row r="176" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A176" s="22">
+      <c r="A176">
         <v>12</v>
       </c>
       <c r="B176" s="1" t="s">
@@ -6381,20 +5607,20 @@
         <v>140</v>
       </c>
       <c r="E176" s="19" t="s">
-        <v>352</v>
+        <v>304</v>
       </c>
       <c r="F176" s="9" t="s">
         <v>186</v>
       </c>
       <c r="G176" s="7" t="s">
-        <v>353</v>
+        <v>305</v>
       </c>
       <c r="H176" s="7" t="s">
-        <v>354</v>
+        <v>306</v>
       </c>
     </row>
     <row r="177" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A177" s="22">
+      <c r="A177">
         <v>13</v>
       </c>
       <c r="B177" s="1" t="s">
@@ -6407,72 +5633,72 @@
         <v>140</v>
       </c>
       <c r="E177" s="19" t="s">
-        <v>352</v>
+        <v>304</v>
       </c>
       <c r="F177" s="9" t="s">
         <v>186</v>
       </c>
       <c r="G177" s="7" t="s">
-        <v>353</v>
+        <v>305</v>
       </c>
       <c r="H177" s="7" t="s">
-        <v>354</v>
+        <v>306</v>
       </c>
     </row>
     <row r="178" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A178" s="22">
+      <c r="A178">
         <v>14</v>
       </c>
       <c r="B178" s="1" t="s">
-        <v>306</v>
+        <v>258</v>
       </c>
       <c r="C178" s="1" t="s">
-        <v>307</v>
+        <v>259</v>
       </c>
       <c r="D178" s="1" t="s">
         <v>147</v>
       </c>
       <c r="E178" s="19" t="s">
-        <v>352</v>
+        <v>304</v>
       </c>
       <c r="F178" s="9" t="s">
         <v>186</v>
       </c>
       <c r="G178" s="7" t="s">
-        <v>353</v>
+        <v>305</v>
       </c>
       <c r="H178" s="7" t="s">
-        <v>354</v>
+        <v>306</v>
       </c>
     </row>
     <row r="179" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A179" s="22">
+      <c r="A179">
         <v>15</v>
       </c>
       <c r="B179" s="1" t="s">
-        <v>308</v>
+        <v>260</v>
       </c>
       <c r="C179" s="1" t="s">
-        <v>309</v>
+        <v>261</v>
       </c>
       <c r="D179" s="1" t="s">
         <v>147</v>
       </c>
       <c r="E179" s="19" t="s">
-        <v>352</v>
+        <v>304</v>
       </c>
       <c r="F179" s="9" t="s">
         <v>186</v>
       </c>
       <c r="G179" s="7" t="s">
-        <v>353</v>
+        <v>305</v>
       </c>
       <c r="H179" s="7" t="s">
-        <v>354</v>
+        <v>306</v>
       </c>
     </row>
     <row r="180" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A180" s="22">
+      <c r="A180">
         <v>16</v>
       </c>
       <c r="B180" s="1" t="s">
@@ -6485,176 +5711,176 @@
         <v>147</v>
       </c>
       <c r="E180" s="19" t="s">
-        <v>352</v>
+        <v>304</v>
       </c>
       <c r="F180" s="9" t="s">
         <v>186</v>
       </c>
       <c r="G180" s="7" t="s">
-        <v>353</v>
+        <v>305</v>
       </c>
       <c r="H180" s="7" t="s">
-        <v>354</v>
+        <v>306</v>
       </c>
     </row>
     <row r="181" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A181" s="22">
+      <c r="A181">
         <v>17</v>
       </c>
       <c r="B181" s="1" t="s">
-        <v>310</v>
+        <v>262</v>
       </c>
       <c r="C181" s="1" t="s">
-        <v>311</v>
+        <v>263</v>
       </c>
       <c r="D181" s="1" t="s">
         <v>147</v>
       </c>
       <c r="E181" s="19" t="s">
-        <v>352</v>
+        <v>304</v>
       </c>
       <c r="F181" s="9" t="s">
         <v>186</v>
       </c>
       <c r="G181" s="7" t="s">
-        <v>353</v>
+        <v>305</v>
       </c>
       <c r="H181" s="7" t="s">
-        <v>354</v>
+        <v>306</v>
       </c>
     </row>
     <row r="182" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A182" s="22">
+      <c r="A182">
         <v>18</v>
       </c>
       <c r="B182" s="1" t="s">
-        <v>312</v>
+        <v>264</v>
       </c>
       <c r="C182" s="1" t="s">
-        <v>313</v>
+        <v>265</v>
       </c>
       <c r="D182" s="1" t="s">
         <v>147</v>
       </c>
       <c r="E182" s="19" t="s">
-        <v>352</v>
+        <v>304</v>
       </c>
       <c r="F182" s="9" t="s">
         <v>186</v>
       </c>
       <c r="G182" s="7" t="s">
-        <v>353</v>
+        <v>305</v>
       </c>
       <c r="H182" s="7" t="s">
-        <v>354</v>
+        <v>306</v>
       </c>
     </row>
     <row r="183" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A183" s="22">
+      <c r="A183">
         <v>19</v>
       </c>
       <c r="B183" s="1" t="s">
-        <v>314</v>
+        <v>266</v>
       </c>
       <c r="C183" s="1" t="s">
-        <v>315</v>
+        <v>267</v>
       </c>
       <c r="D183" s="1" t="s">
         <v>135</v>
       </c>
       <c r="E183" s="19" t="s">
-        <v>352</v>
+        <v>304</v>
       </c>
       <c r="F183" s="9" t="s">
         <v>186</v>
       </c>
       <c r="G183" s="7" t="s">
-        <v>353</v>
+        <v>305</v>
       </c>
       <c r="H183" s="7" t="s">
-        <v>354</v>
+        <v>306</v>
       </c>
     </row>
     <row r="184" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A184" s="22">
+      <c r="A184">
         <v>20</v>
       </c>
       <c r="B184" s="1" t="s">
-        <v>316</v>
+        <v>268</v>
       </c>
       <c r="C184" s="1" t="s">
-        <v>317</v>
+        <v>269</v>
       </c>
       <c r="D184" s="1" t="s">
         <v>154</v>
       </c>
       <c r="E184" s="19" t="s">
-        <v>352</v>
+        <v>304</v>
       </c>
       <c r="F184" s="9" t="s">
         <v>186</v>
       </c>
       <c r="G184" s="7" t="s">
-        <v>353</v>
+        <v>305</v>
       </c>
       <c r="H184" s="7" t="s">
-        <v>354</v>
+        <v>306</v>
       </c>
     </row>
     <row r="185" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A185" s="22">
+      <c r="A185">
         <v>21</v>
       </c>
       <c r="B185" s="1" t="s">
-        <v>318</v>
+        <v>270</v>
       </c>
       <c r="C185" s="1" t="s">
-        <v>319</v>
+        <v>271</v>
       </c>
       <c r="D185" s="1" t="s">
         <v>161</v>
       </c>
       <c r="E185" s="19" t="s">
-        <v>352</v>
+        <v>304</v>
       </c>
       <c r="F185" s="9" t="s">
         <v>186</v>
       </c>
       <c r="G185" s="7" t="s">
-        <v>353</v>
+        <v>305</v>
       </c>
       <c r="H185" s="7" t="s">
-        <v>354</v>
+        <v>306</v>
       </c>
     </row>
     <row r="186" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A186" s="22">
+      <c r="A186">
         <v>22</v>
       </c>
       <c r="B186" s="1" t="s">
-        <v>320</v>
+        <v>272</v>
       </c>
       <c r="C186" s="1" t="s">
-        <v>321</v>
+        <v>273</v>
       </c>
       <c r="D186" s="1" t="s">
         <v>147</v>
       </c>
       <c r="E186" s="19" t="s">
-        <v>352</v>
+        <v>304</v>
       </c>
       <c r="F186" s="9" t="s">
         <v>186</v>
       </c>
       <c r="G186" s="7" t="s">
-        <v>353</v>
+        <v>305</v>
       </c>
       <c r="H186" s="7" t="s">
-        <v>354</v>
+        <v>306</v>
       </c>
     </row>
     <row r="187" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A187" s="22">
+      <c r="A187">
         <v>23</v>
       </c>
       <c r="B187" s="1" t="s">
@@ -6667,46 +5893,46 @@
         <v>135</v>
       </c>
       <c r="E187" s="19" t="s">
-        <v>352</v>
+        <v>304</v>
       </c>
       <c r="F187" s="9" t="s">
         <v>186</v>
       </c>
       <c r="G187" s="7" t="s">
-        <v>353</v>
+        <v>305</v>
       </c>
       <c r="H187" s="7" t="s">
-        <v>354</v>
+        <v>306</v>
       </c>
     </row>
     <row r="188" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A188" s="22">
+      <c r="A188">
         <v>24</v>
       </c>
       <c r="B188" s="1" t="s">
-        <v>322</v>
+        <v>274</v>
       </c>
       <c r="C188" s="1" t="s">
-        <v>323</v>
+        <v>275</v>
       </c>
       <c r="D188" s="1" t="s">
         <v>148</v>
       </c>
       <c r="E188" s="19" t="s">
-        <v>352</v>
+        <v>304</v>
       </c>
       <c r="F188" s="9" t="s">
         <v>186</v>
       </c>
       <c r="G188" s="7" t="s">
-        <v>353</v>
+        <v>305</v>
       </c>
       <c r="H188" s="7" t="s">
-        <v>354</v>
+        <v>306</v>
       </c>
     </row>
     <row r="189" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A189" s="22">
+      <c r="A189">
         <v>25</v>
       </c>
       <c r="B189" s="1" t="s">
@@ -6719,380 +5945,380 @@
         <v>147</v>
       </c>
       <c r="E189" s="19" t="s">
-        <v>352</v>
+        <v>304</v>
       </c>
       <c r="F189" s="9" t="s">
         <v>186</v>
       </c>
       <c r="G189" s="7" t="s">
-        <v>353</v>
+        <v>305</v>
       </c>
       <c r="H189" s="7" t="s">
-        <v>354</v>
+        <v>306</v>
       </c>
     </row>
     <row r="190" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A190" s="22">
+      <c r="A190">
         <v>26</v>
       </c>
       <c r="B190" s="1" t="s">
-        <v>324</v>
+        <v>276</v>
       </c>
       <c r="C190" s="1" t="s">
-        <v>325</v>
+        <v>277</v>
       </c>
       <c r="D190" s="1" t="s">
         <v>148</v>
       </c>
       <c r="E190" s="19" t="s">
-        <v>352</v>
+        <v>304</v>
       </c>
       <c r="F190" s="9" t="s">
         <v>186</v>
       </c>
       <c r="G190" s="7" t="s">
-        <v>353</v>
+        <v>305</v>
       </c>
       <c r="H190" s="7" t="s">
-        <v>354</v>
+        <v>306</v>
       </c>
     </row>
     <row r="191" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A191" s="22">
+      <c r="A191">
         <v>27</v>
       </c>
       <c r="B191" s="1" t="s">
-        <v>326</v>
+        <v>278</v>
       </c>
       <c r="C191" s="1" t="s">
-        <v>327</v>
+        <v>279</v>
       </c>
       <c r="D191" s="1" t="s">
         <v>148</v>
       </c>
       <c r="E191" s="19" t="s">
-        <v>352</v>
+        <v>304</v>
       </c>
       <c r="F191" s="9" t="s">
         <v>186</v>
       </c>
       <c r="G191" s="7" t="s">
-        <v>353</v>
+        <v>305</v>
       </c>
       <c r="H191" s="7" t="s">
-        <v>354</v>
+        <v>306</v>
       </c>
     </row>
     <row r="192" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A192" s="22">
+      <c r="A192">
         <v>28</v>
       </c>
       <c r="B192" s="1" t="s">
-        <v>328</v>
+        <v>280</v>
       </c>
       <c r="C192" s="1" t="s">
-        <v>329</v>
+        <v>281</v>
       </c>
       <c r="D192" s="1" t="s">
         <v>148</v>
       </c>
       <c r="E192" s="19" t="s">
-        <v>352</v>
+        <v>304</v>
       </c>
       <c r="F192" s="9" t="s">
         <v>186</v>
       </c>
       <c r="G192" s="7" t="s">
-        <v>353</v>
+        <v>305</v>
       </c>
       <c r="H192" s="7" t="s">
-        <v>354</v>
+        <v>306</v>
       </c>
     </row>
     <row r="193" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A193" s="22">
+      <c r="A193">
         <v>29</v>
       </c>
       <c r="B193" s="1" t="s">
-        <v>330</v>
+        <v>282</v>
       </c>
       <c r="C193" s="1" t="s">
-        <v>331</v>
+        <v>283</v>
       </c>
       <c r="D193" s="1" t="s">
         <v>137</v>
       </c>
       <c r="E193" s="19" t="s">
-        <v>352</v>
+        <v>304</v>
       </c>
       <c r="F193" s="9" t="s">
         <v>186</v>
       </c>
       <c r="G193" s="7" t="s">
-        <v>353</v>
+        <v>305</v>
       </c>
       <c r="H193" s="7" t="s">
-        <v>354</v>
+        <v>306</v>
       </c>
     </row>
     <row r="194" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A194" s="22">
+      <c r="A194">
         <v>30</v>
       </c>
       <c r="B194" s="1" t="s">
-        <v>332</v>
+        <v>284</v>
       </c>
       <c r="C194" s="1" t="s">
-        <v>333</v>
+        <v>285</v>
       </c>
       <c r="D194" s="1" t="s">
         <v>137</v>
       </c>
       <c r="E194" s="19" t="s">
-        <v>352</v>
+        <v>304</v>
       </c>
       <c r="F194" s="9" t="s">
         <v>186</v>
       </c>
       <c r="G194" s="7" t="s">
-        <v>353</v>
+        <v>305</v>
       </c>
       <c r="H194" s="7" t="s">
-        <v>354</v>
+        <v>306</v>
       </c>
     </row>
     <row r="195" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A195" s="22">
+      <c r="A195">
         <v>31</v>
       </c>
       <c r="B195" s="1" t="s">
-        <v>334</v>
+        <v>286</v>
       </c>
       <c r="C195" s="1" t="s">
-        <v>335</v>
+        <v>287</v>
       </c>
       <c r="D195" s="1" t="s">
         <v>148</v>
       </c>
       <c r="E195" s="19" t="s">
-        <v>352</v>
+        <v>304</v>
       </c>
       <c r="F195" s="9" t="s">
         <v>186</v>
       </c>
       <c r="G195" s="7" t="s">
-        <v>353</v>
+        <v>305</v>
       </c>
       <c r="H195" s="7" t="s">
-        <v>354</v>
+        <v>306</v>
       </c>
     </row>
     <row r="196" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A196" s="22">
+      <c r="A196">
         <v>32</v>
       </c>
       <c r="B196" s="1" t="s">
-        <v>336</v>
+        <v>288</v>
       </c>
       <c r="C196" s="1" t="s">
-        <v>337</v>
+        <v>289</v>
       </c>
       <c r="D196" s="1" t="s">
         <v>148</v>
       </c>
       <c r="E196" s="19" t="s">
-        <v>352</v>
+        <v>304</v>
       </c>
       <c r="F196" s="9" t="s">
         <v>186</v>
       </c>
       <c r="G196" s="7" t="s">
-        <v>353</v>
+        <v>305</v>
       </c>
       <c r="H196" s="7" t="s">
-        <v>354</v>
+        <v>306</v>
       </c>
     </row>
     <row r="197" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A197" s="22">
+      <c r="A197">
         <v>33</v>
       </c>
       <c r="B197" s="1" t="s">
-        <v>338</v>
+        <v>290</v>
       </c>
       <c r="C197" s="1" t="s">
-        <v>339</v>
+        <v>291</v>
       </c>
       <c r="D197" s="1" t="s">
         <v>147</v>
       </c>
       <c r="E197" s="19" t="s">
-        <v>352</v>
+        <v>304</v>
       </c>
       <c r="F197" s="9" t="s">
         <v>186</v>
       </c>
       <c r="G197" s="7" t="s">
-        <v>353</v>
+        <v>305</v>
       </c>
       <c r="H197" s="7" t="s">
-        <v>354</v>
+        <v>306</v>
       </c>
     </row>
     <row r="198" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A198" s="22">
+      <c r="A198">
         <v>34</v>
       </c>
       <c r="B198" s="1" t="s">
-        <v>340</v>
+        <v>292</v>
       </c>
       <c r="C198" s="1" t="s">
-        <v>341</v>
+        <v>293</v>
       </c>
       <c r="D198" s="1" t="s">
         <v>147</v>
       </c>
       <c r="E198" s="19" t="s">
-        <v>352</v>
+        <v>304</v>
       </c>
       <c r="F198" s="9" t="s">
         <v>186</v>
       </c>
       <c r="G198" s="7" t="s">
-        <v>353</v>
+        <v>305</v>
       </c>
       <c r="H198" s="7" t="s">
-        <v>354</v>
+        <v>306</v>
       </c>
     </row>
     <row r="199" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A199" s="22">
+      <c r="A199">
         <v>35</v>
       </c>
       <c r="B199" s="1" t="s">
-        <v>342</v>
+        <v>294</v>
       </c>
       <c r="C199" s="1" t="s">
-        <v>343</v>
+        <v>295</v>
       </c>
       <c r="D199" s="1" t="s">
         <v>147</v>
       </c>
       <c r="E199" s="19" t="s">
-        <v>352</v>
+        <v>304</v>
       </c>
       <c r="F199" s="9" t="s">
         <v>186</v>
       </c>
       <c r="G199" s="7" t="s">
-        <v>353</v>
+        <v>305</v>
       </c>
       <c r="H199" s="7" t="s">
-        <v>354</v>
+        <v>306</v>
       </c>
     </row>
     <row r="200" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A200" s="22">
+      <c r="A200">
         <v>36</v>
       </c>
       <c r="B200" s="1" t="s">
-        <v>344</v>
+        <v>296</v>
       </c>
       <c r="C200" s="1" t="s">
-        <v>345</v>
+        <v>297</v>
       </c>
       <c r="D200" s="1" t="s">
         <v>147</v>
       </c>
       <c r="E200" s="19" t="s">
-        <v>352</v>
+        <v>304</v>
       </c>
       <c r="F200" s="9" t="s">
         <v>186</v>
       </c>
       <c r="G200" s="7" t="s">
-        <v>353</v>
+        <v>305</v>
       </c>
       <c r="H200" s="7" t="s">
-        <v>354</v>
+        <v>306</v>
       </c>
     </row>
     <row r="201" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A201" s="22">
+      <c r="A201">
         <v>37</v>
       </c>
       <c r="B201" s="1" t="s">
-        <v>346</v>
+        <v>298</v>
       </c>
       <c r="C201" s="1" t="s">
-        <v>347</v>
+        <v>299</v>
       </c>
       <c r="D201" s="1" t="s">
         <v>147</v>
       </c>
       <c r="E201" s="19" t="s">
-        <v>352</v>
+        <v>304</v>
       </c>
       <c r="F201" s="9" t="s">
         <v>186</v>
       </c>
       <c r="G201" s="7" t="s">
-        <v>353</v>
+        <v>305</v>
       </c>
       <c r="H201" s="7" t="s">
-        <v>354</v>
+        <v>306</v>
       </c>
     </row>
     <row r="202" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A202" s="22">
+      <c r="A202">
         <v>38</v>
       </c>
       <c r="B202" s="1" t="s">
-        <v>348</v>
+        <v>300</v>
       </c>
       <c r="C202" s="1" t="s">
-        <v>349</v>
+        <v>301</v>
       </c>
       <c r="D202" s="1" t="s">
         <v>147</v>
       </c>
       <c r="E202" s="19" t="s">
-        <v>352</v>
+        <v>304</v>
       </c>
       <c r="F202" s="9" t="s">
         <v>186</v>
       </c>
       <c r="G202" s="7" t="s">
-        <v>353</v>
+        <v>305</v>
       </c>
       <c r="H202" s="7" t="s">
-        <v>354</v>
+        <v>306</v>
       </c>
     </row>
     <row r="203" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A203" s="22">
+      <c r="A203">
         <v>39</v>
       </c>
       <c r="B203" s="1" t="s">
-        <v>350</v>
+        <v>302</v>
       </c>
       <c r="C203" s="1" t="s">
-        <v>351</v>
+        <v>303</v>
       </c>
       <c r="D203" s="1" t="s">
         <v>138</v>
       </c>
       <c r="E203" s="19" t="s">
-        <v>352</v>
+        <v>304</v>
       </c>
       <c r="F203" s="9" t="s">
         <v>186</v>
       </c>
       <c r="G203" s="7" t="s">
-        <v>353</v>
+        <v>305</v>
       </c>
       <c r="H203" s="7" t="s">
-        <v>354</v>
+        <v>306</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
commit comparação de colunas pnad entre trimestres / windows 08112024
</commit_message>
<xml_diff>
--- a/Tabela Variaveis Analises Pe de Meia.xlsx
+++ b/Tabela Variaveis Analises Pe de Meia.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f97fb756bfb044a9/1. Educacao/2. Academia/3. DOUTORADO/USP - Economia Aplicada/MATERIAS/Eco II - Daniel/Desafio Eco II - Pe de Meia/Github/pedemeia3/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f97fb756bfb044a9/1. Educacao/2. Academia/3. DOUTORADO/USP - Economia Aplicada/MATERIAS/Eco II - Daniel/Desafio Eco II - Pe de Meia/Github/pedemeia4/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="159" documentId="8_{F1CD36D2-19BE-47EB-AE65-13017DD7740D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A771D721-A488-4C0A-A884-AAB03392664F}"/>
+  <xr:revisionPtr revIDLastSave="160" documentId="8_{F1CD36D2-19BE-47EB-AE65-13017DD7740D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DAFB6431-8E71-417F-BD21-36B190A8E84E}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{3F24F635-5B38-4FE0-8A30-7E7C7EEBC13B}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Planilha1!$A$1:$H$130</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Planilha1!$A$1:$H$203</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -1590,10 +1590,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{247AA1CF-A420-4D91-B350-1F036DB135E9}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:H203"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="C89" sqref="C89"/>
+    <sheetView tabSelected="1" topLeftCell="A70" workbookViewId="0">
+      <selection activeCell="D93" sqref="D93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1633,7 +1634,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1659,7 +1660,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1686,7 +1687,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1712,7 +1713,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1738,7 +1739,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1764,7 +1765,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1790,7 +1791,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1816,7 +1817,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1842,7 +1843,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1868,7 +1869,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1894,7 +1895,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1920,7 +1921,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1946,7 +1947,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1972,7 +1973,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1998,7 +1999,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>15</v>
       </c>
@@ -2024,7 +2025,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>16</v>
       </c>
@@ -2050,7 +2051,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>17</v>
       </c>
@@ -2076,7 +2077,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>18</v>
       </c>
@@ -2102,7 +2103,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>19</v>
       </c>
@@ -2128,7 +2129,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>20</v>
       </c>
@@ -2154,7 +2155,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>21</v>
       </c>
@@ -2180,7 +2181,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>22</v>
       </c>
@@ -2206,7 +2207,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>23</v>
       </c>
@@ -2232,7 +2233,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>24</v>
       </c>
@@ -2258,7 +2259,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>25</v>
       </c>
@@ -2284,7 +2285,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>26</v>
       </c>
@@ -2310,7 +2311,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>27</v>
       </c>
@@ -2336,7 +2337,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="29" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:8" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>28</v>
       </c>
@@ -2362,7 +2363,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>29</v>
       </c>
@@ -2388,7 +2389,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>30</v>
       </c>
@@ -2414,7 +2415,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="32" spans="1:8" s="10" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:8" s="10" customFormat="1" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A32" s="10">
         <v>31</v>
       </c>
@@ -2440,7 +2441,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>1</v>
       </c>
@@ -2466,7 +2467,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>2</v>
       </c>
@@ -2493,7 +2494,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>3</v>
       </c>
@@ -2519,7 +2520,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>4</v>
       </c>
@@ -2545,7 +2546,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>5</v>
       </c>
@@ -2571,7 +2572,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>6</v>
       </c>
@@ -2597,7 +2598,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>7</v>
       </c>
@@ -2623,7 +2624,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>8</v>
       </c>
@@ -2649,7 +2650,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>9</v>
       </c>
@@ -2675,7 +2676,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>10</v>
       </c>
@@ -2701,7 +2702,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>11</v>
       </c>
@@ -2727,7 +2728,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>12</v>
       </c>
@@ -2753,7 +2754,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>13</v>
       </c>
@@ -2779,7 +2780,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>14</v>
       </c>
@@ -2805,7 +2806,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>15</v>
       </c>
@@ -2831,7 +2832,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>16</v>
       </c>
@@ -2857,7 +2858,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>17</v>
       </c>
@@ -2883,7 +2884,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>18</v>
       </c>
@@ -2909,7 +2910,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>19</v>
       </c>
@@ -2935,7 +2936,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="52" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:8" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>20</v>
       </c>
@@ -2961,7 +2962,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>21</v>
       </c>
@@ -2987,7 +2988,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>22</v>
       </c>
@@ -3013,7 +3014,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>23</v>
       </c>
@@ -3039,7 +3040,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>24</v>
       </c>
@@ -3065,7 +3066,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>25</v>
       </c>
@@ -3091,7 +3092,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>26</v>
       </c>
@@ -3117,7 +3118,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>27</v>
       </c>
@@ -3143,7 +3144,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>28</v>
       </c>
@@ -3169,7 +3170,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>29</v>
       </c>
@@ -3195,7 +3196,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>30</v>
       </c>
@@ -3221,7 +3222,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>31</v>
       </c>
@@ -3247,7 +3248,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>32</v>
       </c>
@@ -3273,7 +3274,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>33</v>
       </c>
@@ -3299,7 +3300,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>34</v>
       </c>
@@ -3325,7 +3326,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="67" spans="1:8" s="10" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:8" s="10" customFormat="1" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A67" s="10">
         <v>35</v>
       </c>
@@ -4693,7 +4694,7 @@
       <c r="G130" s="12"/>
       <c r="H130" s="12"/>
     </row>
-    <row r="131" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A131">
         <v>1</v>
       </c>
@@ -4711,7 +4712,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="132" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A132">
         <v>2</v>
       </c>
@@ -4729,7 +4730,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="133" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A133">
         <v>3</v>
       </c>
@@ -4747,7 +4748,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="134" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A134">
         <v>4</v>
       </c>
@@ -4765,7 +4766,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="135" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A135">
         <v>5</v>
       </c>
@@ -4783,7 +4784,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="136" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A136">
         <v>6</v>
       </c>
@@ -4801,7 +4802,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="137" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A137">
         <v>7</v>
       </c>
@@ -4819,7 +4820,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="138" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A138">
         <v>8</v>
       </c>
@@ -4837,7 +4838,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="139" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A139">
         <v>9</v>
       </c>
@@ -4855,7 +4856,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="140" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A140">
         <v>10</v>
       </c>
@@ -4873,7 +4874,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="141" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A141">
         <v>11</v>
       </c>
@@ -4891,7 +4892,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="142" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A142">
         <v>12</v>
       </c>
@@ -4909,7 +4910,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="143" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A143">
         <v>13</v>
       </c>
@@ -4927,7 +4928,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="144" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A144">
         <v>14</v>
       </c>
@@ -4945,7 +4946,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="145" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A145">
         <v>15</v>
       </c>
@@ -4963,7 +4964,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="146" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A146">
         <v>16</v>
       </c>
@@ -4981,7 +4982,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="147" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A147">
         <v>17</v>
       </c>
@@ -4999,7 +5000,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="148" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A148">
         <v>18</v>
       </c>
@@ -5017,7 +5018,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="149" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A149">
         <v>19</v>
       </c>
@@ -5035,7 +5036,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="150" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:6" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A150">
         <v>20</v>
       </c>
@@ -5053,7 +5054,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="151" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A151">
         <v>21</v>
       </c>
@@ -5071,7 +5072,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="152" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A152">
         <v>22</v>
       </c>
@@ -5089,7 +5090,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="153" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A153">
         <v>23</v>
       </c>
@@ -5107,7 +5108,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="154" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A154">
         <v>24</v>
       </c>
@@ -5125,7 +5126,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="155" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A155">
         <v>25</v>
       </c>
@@ -5143,7 +5144,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="156" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A156">
         <v>26</v>
       </c>
@@ -5161,7 +5162,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="157" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A157">
         <v>27</v>
       </c>
@@ -5179,7 +5180,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="158" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A158">
         <v>28</v>
       </c>
@@ -5197,7 +5198,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="159" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A159">
         <v>29</v>
       </c>
@@ -5215,7 +5216,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="160" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
       <c r="A160">
         <v>30</v>
       </c>
@@ -5233,7 +5234,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="161" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A161">
         <v>31</v>
       </c>
@@ -5251,7 +5252,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="162" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A162">
         <v>32</v>
       </c>
@@ -5269,7 +5270,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="163" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A163">
         <v>33</v>
       </c>
@@ -5287,7 +5288,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="164" spans="1:8" s="10" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="164" spans="1:8" s="10" customFormat="1" ht="15" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A164" s="10">
         <v>34</v>
       </c>
@@ -6322,7 +6323,13 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H130" xr:uid="{247AA1CF-A420-4D91-B350-1F036DB135E9}"/>
+  <autoFilter ref="A1:H203" xr:uid="{247AA1CF-A420-4D91-B350-1F036DB135E9}">
+    <filterColumn colId="5">
+      <filters>
+        <filter val="PNADc"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>

</xml_diff>